<commit_message>
Updated Data driven Login and search scenarios for chrome and firefox
</commit_message>
<xml_diff>
--- a/src/test/java/com/shopclues/testData/Data.xlsx
+++ b/src/test/java/com/shopclues/testData/Data.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63D1F47-6DFF-44A7-B3D1-CA34D5168502}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{805266AD-FB6F-4D2B-80D3-BD0C964032F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="30" windowWidth="14115" windowHeight="15570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="14175" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,10 +57,10 @@
     <t>Nike shoes</t>
   </si>
   <si>
-    <t>Apple iphone</t>
-  </si>
-  <si>
     <t>himalaya baby products</t>
+  </si>
+  <si>
+    <t>Sunglasses</t>
   </si>
 </sst>
 </file>
@@ -551,12 +552,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>